<commit_message>
first batch of examples
</commit_message>
<xml_diff>
--- a/datasets/sdg_separates/UN-examples/description.xlsx
+++ b/datasets/sdg_separates/UN-examples/description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlafleur/Projects/SDG-samples/datasets/sdg_separates/UN-examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CD6999-65CB-4841-BD12-D0223E8A95FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1702183E-D737-1947-8C9E-9D94BA0DD77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{24A97125-F1E0-C449-ADA9-A4C46189A366}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t xml:space="preserve"> Description of data files</t>
   </si>
@@ -120,13 +120,25 @@
   </si>
   <si>
     <t>https://www.unescap.org/sites/default/files/SDG_01_ESCAP_SYB2016_SDG_baseline_report.pdf</t>
+  </si>
+  <si>
+    <t>https://unstats.un.org/sdgs/files/report/2018/secretary-general-sdg-report-2018--en.pdf</t>
+  </si>
+  <si>
+    <t>This is from the "Progress towards the Sustainable Development Goals Report of the Secretary-General"</t>
+  </si>
+  <si>
+    <t>https://hlpf.un.org/2017/inputs-to-the-hlpf-background-notes</t>
+  </si>
+  <si>
+    <t>HLPF reviews (subset of sdgs in different years)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,6 +168,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Whitney"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -184,12 +201,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -505,29 +523,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B7F3B7-6699-F642-942F-65992B6C1413}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -535,7 +553,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -543,7 +561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -551,7 +569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -559,7 +577,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -567,15 +585,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -583,15 +604,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -599,7 +623,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -607,7 +631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -615,7 +639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -623,7 +647,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -631,24 +655,48 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B16" r:id="rId1" xr:uid="{6D6955A9-9DB2-7A44-BE2B-D0C7404CA0AD}"/>
     <hyperlink ref="B18" r:id="rId2" xr:uid="{79667081-1AD9-574F-B462-55A430BC6BE8}"/>
+    <hyperlink ref="C11" r:id="rId3" xr:uid="{D733B8D0-A4F4-304C-9D18-F759ACD87B7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>